<commit_message>
update id schema effective date
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Mosip Codebase\GUINEA_Pilot\GUINEA_Pilot_Mosip-Data_WuriGuinea-1.2.0.1-B1\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicroTech\IdeaProjects\mosip-data-guinea\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B2447C-8FFA-4770-B918-12349467D142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E71D605-A46F-4968-B07B-A6827368F45D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -577,7 +577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -936,17 +936,19 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="22.90625" customWidth="1"/>
-    <col min="6" max="6" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="6" max="6" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -996,7 +998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1019,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2">
-        <v>3.6071759259259262E-2</v>
+        <v>45079.634583333333</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
@@ -1031,7 +1033,7 @@
         <v>15</v>
       </c>
       <c r="L2" s="2">
-        <v>3.6047453703703707E-2</v>
+        <v>45079.634583333333</v>
       </c>
       <c r="M2" t="s">
         <v>22</v>

</xml_diff>